<commit_message>
Adjustment for hourly resolution optimization
</commit_message>
<xml_diff>
--- a/hypatia/examples/Planning_teaching/sets/global.xlsx
+++ b/hypatia/examples/Planning_teaching/sets/global.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="172" documentId="13_ncr:1_{46DC28F1-8408-4275-A816-F6E488DFF122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1439A3A-7E25-4D19-8F45-64C89BA535A2}"/>
+  <xr:revisionPtr revIDLastSave="180" documentId="13_ncr:1_{46DC28F1-8408-4275-A816-F6E488DFF122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D5C97B70-1E8A-4F2C-83D5-938E92FCA558}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1490" yWindow="1490" windowWidth="14380" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="6500" yWindow="1700" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sets" sheetId="1" r:id="rId1"/>
@@ -559,12 +559,8 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1055,7 +1051,7 @@
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Timeslice" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Timeslice_name" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Timeslice_fraction" dataDxfId="0">
-      <calculatedColumnFormula>1/8760</calculatedColumnFormula>
+      <calculatedColumnFormula>0.000114155251141553*365</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1339,8 +1335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2035,7 +2031,7 @@
         <v>23</v>
       </c>
       <c r="C61" s="11">
-        <v>1.1415525114155251E-4</v>
+        <v>4.1666666666666803E-2</v>
       </c>
       <c r="E61" s="9"/>
     </row>
@@ -2047,7 +2043,7 @@
         <v>24</v>
       </c>
       <c r="C62" s="11">
-        <v>1.1415525114155251E-4</v>
+        <v>4.1666666666666845E-2</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.35">
@@ -2058,7 +2054,7 @@
         <v>25</v>
       </c>
       <c r="C63" s="11">
-        <v>1.1415525114155251E-4</v>
+        <v>4.1666666666666845E-2</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.35">
@@ -2069,7 +2065,7 @@
         <v>26</v>
       </c>
       <c r="C64" s="11">
-        <v>1.1415525114155251E-4</v>
+        <v>4.1666666666666845E-2</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
@@ -2080,7 +2076,7 @@
         <v>27</v>
       </c>
       <c r="C65" s="11">
-        <v>1.1415525114155251E-4</v>
+        <v>4.1666666666666845E-2</v>
       </c>
       <c r="E65" s="9"/>
     </row>
@@ -2092,7 +2088,7 @@
         <v>28</v>
       </c>
       <c r="C66" s="11">
-        <v>1.1415525114155251E-4</v>
+        <v>4.1666666666666845E-2</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
@@ -2103,7 +2099,7 @@
         <v>29</v>
       </c>
       <c r="C67" s="11">
-        <v>1.1415525114155251E-4</v>
+        <v>4.1666666666666845E-2</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
@@ -2114,7 +2110,7 @@
         <v>30</v>
       </c>
       <c r="C68" s="11">
-        <v>1.1415525114155251E-4</v>
+        <v>4.1666666666666845E-2</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
@@ -2125,7 +2121,7 @@
         <v>31</v>
       </c>
       <c r="C69" s="11">
-        <v>1.1415525114155251E-4</v>
+        <v>4.1666666666666845E-2</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
@@ -2136,7 +2132,7 @@
         <v>32</v>
       </c>
       <c r="C70" s="11">
-        <v>1.1415525114155251E-4</v>
+        <v>4.1666666666666845E-2</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
@@ -2147,7 +2143,7 @@
         <v>33</v>
       </c>
       <c r="C71" s="11">
-        <v>1.1415525114155251E-4</v>
+        <v>4.1666666666666845E-2</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
@@ -2158,7 +2154,7 @@
         <v>34</v>
       </c>
       <c r="C72" s="11">
-        <v>1.1415525114155251E-4</v>
+        <v>4.1666666666666845E-2</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
@@ -2169,7 +2165,7 @@
         <v>35</v>
       </c>
       <c r="C73" s="11">
-        <v>1.1415525114155251E-4</v>
+        <v>4.1666666666666845E-2</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
@@ -2180,7 +2176,7 @@
         <v>36</v>
       </c>
       <c r="C74" s="11">
-        <v>1.1415525114155251E-4</v>
+        <v>4.1666666666666845E-2</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
@@ -2191,7 +2187,7 @@
         <v>37</v>
       </c>
       <c r="C75" s="11">
-        <v>1.1415525114155251E-4</v>
+        <v>4.1666666666666845E-2</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
@@ -2202,7 +2198,7 @@
         <v>38</v>
       </c>
       <c r="C76" s="11">
-        <v>1.1415525114155251E-4</v>
+        <v>4.1666666666666845E-2</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.35">
@@ -2213,7 +2209,7 @@
         <v>39</v>
       </c>
       <c r="C77" s="11">
-        <v>1.1415525114155251E-4</v>
+        <v>4.1666666666666845E-2</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.35">
@@ -2224,7 +2220,7 @@
         <v>40</v>
       </c>
       <c r="C78" s="11">
-        <v>1.1415525114155251E-4</v>
+        <v>4.1666666666666845E-2</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.35">
@@ -2235,7 +2231,7 @@
         <v>41</v>
       </c>
       <c r="C79" s="11">
-        <v>1.1415525114155251E-4</v>
+        <v>4.1666666666666845E-2</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.35">
@@ -2246,7 +2242,7 @@
         <v>42</v>
       </c>
       <c r="C80" s="11">
-        <v>1.1415525114155251E-4</v>
+        <v>4.1666666666666845E-2</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
@@ -2257,7 +2253,7 @@
         <v>43</v>
       </c>
       <c r="C81" s="11">
-        <v>1.1415525114155251E-4</v>
+        <v>4.1666666666666845E-2</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
@@ -2268,7 +2264,7 @@
         <v>44</v>
       </c>
       <c r="C82" s="11">
-        <v>1.1415525114155251E-4</v>
+        <v>4.1666666666666845E-2</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
@@ -2279,7 +2275,7 @@
         <v>45</v>
       </c>
       <c r="C83" s="11">
-        <v>1.1415525114155251E-4</v>
+        <v>4.1666666666666845E-2</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
@@ -2290,7 +2286,7 @@
         <v>46</v>
       </c>
       <c r="C84" s="11">
-        <v>1.1415525114155251E-4</v>
+        <v>4.1666666666666845E-2</v>
       </c>
     </row>
   </sheetData>
@@ -2552,6 +2548,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="5d44ae6a-e145-4c9d-94e7-ddf9cc58067e">
@@ -2568,15 +2573,6 @@
     </SharedWithUsers>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2599,6 +2595,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{400CE890-4FAA-43FF-AB05-78D100D91AC8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82347752-6D50-4565-8A47-C3BD006EDCEE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -2607,12 +2611,4 @@
     <ds:schemaRef ds:uri="e67e9a88-35e1-4b39-8da9-a609eb308282"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{400CE890-4FAA-43FF-AB05-78D100D91AC8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>